<commit_message>
added humiport for synop obs plot
</commit_message>
<xml_diff>
--- a/data/excel/syn_obs_template.xlsx
+++ b/data/excel/syn_obs_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14960" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25680" windowHeight="14960" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Blatt1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>MESZ</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>Td_davis-station</t>
+  </si>
+  <si>
+    <t>T_humiport</t>
+  </si>
+  <si>
+    <t>RH_humiport</t>
   </si>
 </sst>
 </file>
@@ -145,8 +151,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -164,17 +174,21 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="15">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -504,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y16"/>
+  <dimension ref="A1:AA16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -527,17 +541,19 @@
     <col min="14" max="14" width="8.83203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.83203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="23" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15" customWidth="1"/>
+    <col min="18" max="18" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="25" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:27">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -590,31 +606,37 @@
         <v>24</v>
       </c>
       <c r="R1" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" t="s">
+        <v>26</v>
+      </c>
+      <c r="T1" t="s">
         <v>11</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>12</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>13</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>14</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>15</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>16</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>17</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:25">
+    <row r="2" spans="1:27">
       <c r="A2" s="1">
         <v>0.20833333333333334</v>
       </c>
@@ -667,29 +689,35 @@
         <v>10.5</v>
       </c>
       <c r="R2" s="2">
+        <v>11</v>
+      </c>
+      <c r="S2" s="2">
+        <v>85</v>
+      </c>
+      <c r="T2" s="2">
         <v>918.8</v>
       </c>
-      <c r="S2" s="2">
+      <c r="U2" s="2">
         <v>0.9</v>
       </c>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3">
+      <c r="V2" s="3"/>
+      <c r="W2" s="3">
         <v>9</v>
       </c>
-      <c r="V2" s="3">
+      <c r="X2" s="3">
         <v>6</v>
       </c>
-      <c r="W2" s="3">
+      <c r="Y2" s="3">
         <v>30</v>
       </c>
-      <c r="X2" s="3">
+      <c r="Z2" s="3">
         <v>7</v>
       </c>
-      <c r="Y2" s="3">
+      <c r="AA2" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:25">
+    <row r="3" spans="1:27">
       <c r="A3" s="1">
         <v>0.25</v>
       </c>
@@ -742,27 +770,33 @@
         <v>11.3</v>
       </c>
       <c r="R3" s="2">
+        <v>11</v>
+      </c>
+      <c r="S3" s="2">
+        <v>90</v>
+      </c>
+      <c r="T3" s="2">
         <v>918.7</v>
       </c>
-      <c r="S3" s="2">
+      <c r="U3" s="2">
         <v>0.8</v>
       </c>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3">
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3">
         <v>6</v>
       </c>
-      <c r="W3" s="3">
+      <c r="Y3" s="3">
         <v>20</v>
       </c>
-      <c r="X3" s="3">
+      <c r="Z3" s="3">
         <v>8</v>
       </c>
-      <c r="Y3" s="3">
+      <c r="AA3" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:25">
+    <row r="4" spans="1:27">
       <c r="A4" s="1">
         <v>0.29166666666666669</v>
       </c>
@@ -815,27 +849,33 @@
         <v>11.4</v>
       </c>
       <c r="R4" s="2">
+        <v>11</v>
+      </c>
+      <c r="S4" s="2">
+        <v>91</v>
+      </c>
+      <c r="T4" s="2">
         <v>918.9</v>
       </c>
-      <c r="S4" s="2">
+      <c r="U4" s="2">
         <v>0.8</v>
       </c>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3">
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3">
         <v>6</v>
       </c>
-      <c r="W4" s="3">
+      <c r="Y4" s="3">
         <v>20</v>
       </c>
-      <c r="X4" s="3">
+      <c r="Z4" s="3">
         <v>8</v>
       </c>
-      <c r="Y4" s="3">
+      <c r="AA4" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:25">
+    <row r="5" spans="1:27">
       <c r="A5" s="1">
         <v>0.33333333333333331</v>
       </c>
@@ -888,29 +928,35 @@
         <v>11.5</v>
       </c>
       <c r="R5" s="2">
+        <v>12</v>
+      </c>
+      <c r="S5" s="2">
+        <v>90</v>
+      </c>
+      <c r="T5" s="2">
         <v>919</v>
       </c>
-      <c r="S5" s="2">
+      <c r="U5" s="2">
         <v>0.9</v>
       </c>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3">
+      <c r="V5" s="3"/>
+      <c r="W5" s="3">
         <v>4</v>
       </c>
-      <c r="V5" s="3">
+      <c r="X5" s="3">
         <v>6</v>
       </c>
-      <c r="W5" s="3">
+      <c r="Y5" s="3">
         <v>30</v>
       </c>
-      <c r="X5" s="3">
+      <c r="Z5" s="3">
         <v>7</v>
       </c>
-      <c r="Y5" s="3">
+      <c r="AA5" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:25">
+    <row r="6" spans="1:27">
       <c r="A6" s="1">
         <v>0.375</v>
       </c>
@@ -963,23 +1009,29 @@
         <v>11.3</v>
       </c>
       <c r="R6" s="2">
+        <v>13</v>
+      </c>
+      <c r="S6" s="2">
+        <v>85</v>
+      </c>
+      <c r="T6" s="2">
         <v>919.1</v>
       </c>
-      <c r="S6" s="2">
+      <c r="U6" s="2">
         <v>1.5</v>
       </c>
-      <c r="T6" s="3"/>
-      <c r="U6" s="3"/>
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
-      <c r="X6" s="3">
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3">
         <v>0</v>
       </c>
-      <c r="Y6" s="3">
+      <c r="AA6" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:25">
+    <row r="7" spans="1:27">
       <c r="A7" s="1">
         <v>0.41666666666666669</v>
       </c>
@@ -1032,23 +1084,29 @@
         <v>11.5</v>
       </c>
       <c r="R7" s="2">
+        <v>14</v>
+      </c>
+      <c r="S7" s="2">
+        <v>81</v>
+      </c>
+      <c r="T7" s="2">
         <v>918.8</v>
       </c>
-      <c r="S7" s="2">
+      <c r="U7" s="2">
         <v>3</v>
       </c>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3"/>
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
-      <c r="X7" s="3">
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3">
         <v>0</v>
       </c>
-      <c r="Y7" s="3">
+      <c r="AA7" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:25">
+    <row r="8" spans="1:27">
       <c r="A8" s="1">
         <v>0.45833333333333331</v>
       </c>
@@ -1101,23 +1159,29 @@
         <v>11.9</v>
       </c>
       <c r="R8" s="2">
+        <v>16</v>
+      </c>
+      <c r="S8" s="2">
+        <v>70</v>
+      </c>
+      <c r="T8" s="2">
         <v>918.5</v>
       </c>
-      <c r="S8" s="2">
+      <c r="U8" s="2">
         <v>4.5</v>
       </c>
-      <c r="T8" s="3"/>
-      <c r="U8" s="3"/>
       <c r="V8" s="3"/>
       <c r="W8" s="3"/>
-      <c r="X8" s="3">
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3">
         <v>0</v>
       </c>
-      <c r="Y8" s="3">
+      <c r="AA8" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:25">
+    <row r="9" spans="1:27">
       <c r="A9" s="1">
         <v>0.5</v>
       </c>
@@ -1170,27 +1234,33 @@
         <v>12.2</v>
       </c>
       <c r="R9" s="2">
+        <v>14</v>
+      </c>
+      <c r="S9" s="2">
+        <v>70</v>
+      </c>
+      <c r="T9" s="2">
         <v>918.8</v>
       </c>
-      <c r="S9" s="2">
+      <c r="U9" s="2">
         <v>4.5</v>
       </c>
-      <c r="T9" s="3"/>
-      <c r="U9" s="3"/>
-      <c r="V9" s="3">
-        <v>8</v>
-      </c>
-      <c r="W9" s="3">
-        <v>750</v>
-      </c>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
       <c r="X9" s="3">
         <v>8</v>
       </c>
       <c r="Y9" s="3">
+        <v>750</v>
+      </c>
+      <c r="Z9" s="3">
         <v>8</v>
       </c>
+      <c r="AA9" s="3">
+        <v>8</v>
+      </c>
     </row>
-    <row r="10" spans="1:25">
+    <row r="10" spans="1:27">
       <c r="A10" s="1">
         <v>0.54166666666666663</v>
       </c>
@@ -1243,29 +1313,35 @@
         <v>12.5</v>
       </c>
       <c r="R10" s="2">
+        <v>14</v>
+      </c>
+      <c r="S10" s="2">
+        <v>75</v>
+      </c>
+      <c r="T10" s="2">
         <v>918.8</v>
       </c>
-      <c r="S10" s="2">
+      <c r="U10" s="2">
         <v>5</v>
       </c>
-      <c r="T10" s="3"/>
-      <c r="U10" s="3">
+      <c r="V10" s="3"/>
+      <c r="W10" s="3">
         <v>7</v>
-      </c>
-      <c r="V10" s="3">
-        <v>8</v>
-      </c>
-      <c r="W10" s="3">
-        <v>1100</v>
       </c>
       <c r="X10" s="3">
         <v>8</v>
       </c>
       <c r="Y10" s="3">
+        <v>1100</v>
+      </c>
+      <c r="Z10" s="3">
+        <v>8</v>
+      </c>
+      <c r="AA10" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:25">
+    <row r="11" spans="1:27">
       <c r="A11" s="1">
         <v>0.58333333333333337</v>
       </c>
@@ -1318,27 +1394,33 @@
         <v>12.6</v>
       </c>
       <c r="R11" s="2">
+        <v>16</v>
+      </c>
+      <c r="S11" s="2">
+        <v>70</v>
+      </c>
+      <c r="T11" s="2">
         <v>918.7</v>
       </c>
-      <c r="S11" s="2">
+      <c r="U11" s="2">
         <v>5</v>
       </c>
-      <c r="T11" s="3"/>
-      <c r="U11" s="3"/>
-      <c r="V11" s="3">
-        <v>8</v>
-      </c>
-      <c r="W11" s="3">
-        <v>800</v>
-      </c>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
       <c r="X11" s="3">
         <v>8</v>
       </c>
       <c r="Y11" s="3">
+        <v>800</v>
+      </c>
+      <c r="Z11" s="3">
         <v>8</v>
       </c>
+      <c r="AA11" s="3">
+        <v>8</v>
+      </c>
     </row>
-    <row r="12" spans="1:25">
+    <row r="12" spans="1:27">
       <c r="A12" s="1">
         <v>0.625</v>
       </c>
@@ -1391,27 +1473,33 @@
         <v>12.9</v>
       </c>
       <c r="R12" s="2">
+        <v>16</v>
+      </c>
+      <c r="S12" s="2">
+        <v>70</v>
+      </c>
+      <c r="T12" s="2">
         <v>918.1</v>
       </c>
-      <c r="S12" s="2">
+      <c r="U12" s="2">
         <v>4.5</v>
       </c>
-      <c r="T12" s="3"/>
-      <c r="U12" s="3"/>
-      <c r="V12" s="3">
-        <v>8</v>
-      </c>
-      <c r="W12" s="3">
-        <v>900</v>
-      </c>
+      <c r="V12" s="3"/>
+      <c r="W12" s="3"/>
       <c r="X12" s="3">
         <v>8</v>
       </c>
       <c r="Y12" s="3">
+        <v>900</v>
+      </c>
+      <c r="Z12" s="3">
         <v>8</v>
       </c>
+      <c r="AA12" s="3">
+        <v>8</v>
+      </c>
     </row>
-    <row r="13" spans="1:25">
+    <row r="13" spans="1:27">
       <c r="A13" s="1">
         <v>0.66666666666666663</v>
       </c>
@@ -1464,27 +1552,33 @@
         <v>12.4</v>
       </c>
       <c r="R13" s="2">
+        <v>17</v>
+      </c>
+      <c r="S13" s="2">
+        <v>60</v>
+      </c>
+      <c r="T13" s="2">
         <v>917.5</v>
       </c>
-      <c r="S13" s="2">
+      <c r="U13" s="2">
         <v>4.5</v>
       </c>
-      <c r="T13" s="3">
+      <c r="V13" s="3">
         <v>1</v>
       </c>
-      <c r="U13" s="3"/>
-      <c r="V13" s="3"/>
-      <c r="W13" s="3">
+      <c r="W13" s="3"/>
+      <c r="X13" s="3"/>
+      <c r="Y13" s="3">
         <v>4000</v>
       </c>
-      <c r="X13" s="3">
+      <c r="Z13" s="3">
         <v>7</v>
       </c>
-      <c r="Y13" s="3">
+      <c r="AA13" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:25">
+    <row r="14" spans="1:27">
       <c r="A14" s="1">
         <v>0.70833333333333337</v>
       </c>
@@ -1537,27 +1631,33 @@
         <v>14.1</v>
       </c>
       <c r="R14" s="2">
+        <v>17</v>
+      </c>
+      <c r="S14" s="2">
+        <v>65</v>
+      </c>
+      <c r="T14" s="2">
         <v>917.4</v>
       </c>
-      <c r="S14" s="2">
+      <c r="U14" s="2">
         <v>4.5</v>
       </c>
-      <c r="T14" s="3"/>
-      <c r="U14" s="3"/>
-      <c r="V14" s="3">
+      <c r="V14" s="3"/>
+      <c r="W14" s="3"/>
+      <c r="X14" s="3">
         <v>8</v>
       </c>
-      <c r="W14" s="3">
+      <c r="Y14" s="3">
         <v>1100</v>
       </c>
-      <c r="X14" s="3">
+      <c r="Z14" s="3">
         <v>7</v>
       </c>
-      <c r="Y14" s="3">
+      <c r="AA14" s="3">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:25">
+    <row r="15" spans="1:27">
       <c r="A15" s="1">
         <v>0.75</v>
       </c>
@@ -1610,29 +1710,35 @@
         <v>14.9</v>
       </c>
       <c r="R15" s="2">
+        <v>17</v>
+      </c>
+      <c r="S15" s="2">
+        <v>60</v>
+      </c>
+      <c r="T15" s="2">
         <v>916.8</v>
       </c>
-      <c r="S15" s="2">
+      <c r="U15" s="2">
         <v>4.5</v>
       </c>
-      <c r="T15" s="3">
+      <c r="V15" s="3">
         <v>1</v>
       </c>
-      <c r="U15" s="3"/>
-      <c r="V15" s="3">
+      <c r="W15" s="3"/>
+      <c r="X15" s="3">
         <v>8</v>
       </c>
-      <c r="W15" s="3">
+      <c r="Y15" s="3">
         <v>1200</v>
       </c>
-      <c r="X15" s="3">
+      <c r="Z15" s="3">
         <v>7</v>
       </c>
-      <c r="Y15" s="3">
+      <c r="AA15" s="3">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:25">
+    <row r="16" spans="1:27">
       <c r="A16" s="1">
         <v>0.79166666666666663</v>
       </c>
@@ -1685,25 +1791,31 @@
         <v>15.1</v>
       </c>
       <c r="R16" s="2">
+        <v>17</v>
+      </c>
+      <c r="S16" s="2">
+        <v>55</v>
+      </c>
+      <c r="T16" s="2">
         <v>916.1</v>
       </c>
-      <c r="S16" s="2">
+      <c r="U16" s="2">
         <v>4.5</v>
       </c>
-      <c r="T16" s="3">
+      <c r="V16" s="3">
         <v>1</v>
       </c>
-      <c r="U16" s="3"/>
-      <c r="V16" s="3">
+      <c r="W16" s="3"/>
+      <c r="X16" s="3">
         <v>5</v>
       </c>
-      <c r="W16" s="3">
+      <c r="Y16" s="3">
         <v>1500</v>
       </c>
-      <c r="X16" s="3">
+      <c r="Z16" s="3">
         <v>6</v>
       </c>
-      <c r="Y16" s="3">
+      <c r="AA16" s="3">
         <v>5</v>
       </c>
     </row>

</xml_diff>